<commit_message>
denmaerk excel changes for osprey uk
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeadk.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreyemeadk.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8D3C2B-7822-4FE3-939D-BFE7EEFC9810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF8E122-D00F-467A-B8A0-671BD843127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="283">
   <si>
     <t>UserName</t>
   </si>
@@ -892,6 +892,18 @@
   </si>
   <si>
     <t xml:space="preserve">STONEWASH BLACK </t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>abogi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Abcd@123</t>
+  </si>
+  <si>
+    <t>Sjælland</t>
   </si>
 </sst>
 </file>
@@ -3299,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDE721-2994-4A91-8C89-FADAE76105D8}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3414,16 +3426,16 @@
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3443,7 +3455,7 @@
         <v>187</v>
       </c>
       <c r="O2" t="s">
-        <v>185</v>
+        <v>282</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>188</v>
@@ -3479,8 +3491,8 @@
       <c r="A4" t="s">
         <v>99</v>
       </c>
-      <c r="W4" t="s">
-        <v>194</v>
+      <c r="W4" s="5" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -3843,19 +3855,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{C94C20D5-4494-4663-8D15-E3F04F8BA838}"/>
-    <hyperlink ref="D2" r:id="rId2" display="Testers@278" xr:uid="{0F1A9542-CB17-4A46-B151-3CB4195FE686}"/>
-    <hyperlink ref="E2" r:id="rId3" display="Testers@278" xr:uid="{3D6B96F7-7492-4831-BA08-1EC319F3C995}"/>
-    <hyperlink ref="C2" r:id="rId4" display="testersemail.278@gmail.com" xr:uid="{FF5CC51C-5AD9-4693-981E-E7B0E9E657C5}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{D61594FB-34B8-48FF-8601-E5E62BE99A50}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{5D1A5D25-CA74-4312-B274-A09F60758C65}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{05504D73-D67C-47D1-B503-0C5ECD72787A}"/>
-    <hyperlink ref="C13" r:id="rId8" display="testersemail.278@gmail.com" xr:uid="{2FD31558-C54F-4C20-BA79-E4495F4F8A25}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{642BE6BD-6769-4684-BDF3-6EE93DC03E40}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{B56CD3AB-3EF7-427B-AEE9-EFCCB446AE2B}"/>
-    <hyperlink ref="C15" r:id="rId11" xr:uid="{13574855-564B-42A8-BC07-0BB732D28542}"/>
-    <hyperlink ref="B16" r:id="rId12" xr:uid="{4F884725-7BD6-4040-9EB4-E29F2ED09129}"/>
-    <hyperlink ref="C16" r:id="rId13" xr:uid="{50B14846-390B-41D6-AC9B-F1AB298F8D8C}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0F1A9542-CB17-4A46-B151-3CB4195FE686}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{3D6B96F7-7492-4831-BA08-1EC319F3C995}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{FF5CC51C-5AD9-4693-981E-E7B0E9E657C5}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{D61594FB-34B8-48FF-8601-E5E62BE99A50}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{5D1A5D25-CA74-4312-B274-A09F60758C65}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{05504D73-D67C-47D1-B503-0C5ECD72787A}"/>
+    <hyperlink ref="C13" r:id="rId7" display="testersemail.278@gmail.com" xr:uid="{2FD31558-C54F-4C20-BA79-E4495F4F8A25}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{642BE6BD-6769-4684-BDF3-6EE93DC03E40}"/>
+    <hyperlink ref="B15" r:id="rId9" xr:uid="{B56CD3AB-3EF7-427B-AEE9-EFCCB446AE2B}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{13574855-564B-42A8-BC07-0BB732D28542}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{4F884725-7BD6-4040-9EB4-E29F2ED09129}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{50B14846-390B-41D6-AC9B-F1AB298F8D8C}"/>
+    <hyperlink ref="B2" r:id="rId13" xr:uid="{C94C20D5-4494-4663-8D15-E3F04F8BA838}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -3866,7 +3878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B948743-CA29-4DBC-9182-9AC6052C14C8}">
   <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>